<commit_message>
Mejoras al netobook 5, tanto en los textos como en el cálculo.
</commit_message>
<xml_diff>
--- a/data/20201012_sofr_zero.xlsx
+++ b/data/20201012_sofr_zero.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvarodiaz/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvarodiaz/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CBFB98-7003-5B49-8878-08B6D8CE54F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150526F1-49E9-C141-AEA5-F2DB6CA37270}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,7 +432,7 @@
     <t>1Y</t>
   </si>
   <si>
-    <t>SHORTBACK</t>
+    <t>SHORTFRONT</t>
   </si>
 </sst>
 </file>
@@ -3788,7 +3788,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C34"/>
+      <selection activeCell="F2" sqref="F2:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>